<commit_message>
fixes following milena's reviews
</commit_message>
<xml_diff>
--- a/post_hoc_milena/Confounds_list_Milena_v3.xlsx
+++ b/post_hoc_milena/Confounds_list_Milena_v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/roshan-prakash_rane_charite_de/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B99BC64E-3536-4D96-A341-4C686508E449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C60C3F9E-E4E7-402A-85E8-3752B93C1CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="0" windowWidth="28040" windowHeight="17440" xr2:uid="{34A9CFC4-A7AB-7E4E-9272-A74BAF27F8B5}"/>
   </bookViews>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="289">
   <si>
     <t>subject</t>
   </si>
@@ -192,7 +192,7 @@
     <t>8c</t>
   </si>
   <si>
-    <t>median</t>
+    <t>mean</t>
   </si>
   <si>
     <t>Alcohol</t>
@@ -414,7 +414,7 @@
     <t>/BL/psytools/IMAGEN-IMGN_PDS_RC5-IMAGEN_DIGEST.csv</t>
   </si>
   <si>
-    <t>recode a12a_f: 0 = 1, 1 = 4; sum score = a8_f + a9_f + a10_f + a11_f + a12a_f + a13_f + a8_m + a9_m + a10_m + a11_m + a12a_m + a13_m</t>
+    <t>recode a12a_f: 0 = 1, 1 = 4; sum score = a8_f + a9_f + a10_f + a11_f + a12a_f + a13_f + a8_m + a9_m + a10_m + a11_m + a12_m + a13_m</t>
   </si>
   <si>
     <t>Medical</t>
@@ -447,16 +447,28 @@
     <t>sum score 'victim': bully01 + bully02 + bully03 + bully04 + bully09 + bully10</t>
   </si>
   <si>
-    <t>Social_behavior</t>
+    <t>Social_difficulties</t>
   </si>
   <si>
     <t>all_SDQ.csv</t>
   </si>
   <si>
-    <t>/BL/dawba/IMAGEN_dawba_BL.tsv</t>
-  </si>
-  <si>
-    <t>recode items sobeys, sreflect, sattends, sfriend, spopular: 0 = 2, 1 = 1, 2 = 0; sum score = sconsid +  srestles + ssomatic + sshares + stantrum + sloner + sobeys + sworries + scaring + sfidgety + sfriend + sfights + sunhappy + spopular + sdistrac + sclingy + skind + slies + sbullied + shelpout + sreflect + ssteals + soldbest + safraid + sattends + sebddiff + schronic + sdistres + simphome + simpfrie + simpclas + simpleis + sburden + sebdtot + semotion + sconduct + shyper + speer + sprosoc + simpact</t>
+    <t>/FU3/dawba/IMAGEN_dawba_BL.tsv</t>
+  </si>
+  <si>
+    <t>sebdtot</t>
+  </si>
+  <si>
+    <t>Social_difficulties_impact</t>
+  </si>
+  <si>
+    <t>simpact</t>
+  </si>
+  <si>
+    <t>Prosocial_behavior</t>
+  </si>
+  <si>
+    <t>sprosoc</t>
   </si>
   <si>
     <t>Alc_lastmnt_TLFB</t>
@@ -472,9 +484,6 @@
   </si>
   <si>
     <t>tlfb_alcohol1</t>
-  </si>
-  <si>
-    <t>???</t>
   </si>
   <si>
     <t>Tobacco_lastmnt_TLFB</t>
@@ -916,7 +925,7 @@
     <t>Conflict_tactics_parent_mean_psych_aggr</t>
   </si>
   <si>
-    <t>Parent Psychological Agreesion Mean</t>
+    <t>Parent Psychological Agression Mean</t>
   </si>
   <si>
     <t>cts_psychological_aggression</t>
@@ -937,7 +946,7 @@
     <t>all_GEN.csv</t>
   </si>
   <si>
-    <t>Parent Psychiatric Disorders History'</t>
+    <t>Parent Psychiatric Disorders History</t>
   </si>
   <si>
     <t>/BL/psytools/IMAGEN-IMGN_GEN_RC5-BASIC_DIGEST.csv</t>
@@ -1406,17 +1415,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC2DA8B6-DFEF-5842-9AB2-045734C39BBA}">
-  <dimension ref="A1:K130"/>
+  <dimension ref="A1:K135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="C129" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
-    <col min="3" max="3" width="23.25" customWidth="1"/>
+    <col min="3" max="3" width="43.625" customWidth="1"/>
     <col min="4" max="4" width="25.875" customWidth="1"/>
-    <col min="5" max="5" width="17.125" customWidth="1"/>
+    <col min="5" max="5" width="42.125" customWidth="1"/>
     <col min="6" max="6" width="60.625" customWidth="1"/>
     <col min="7" max="7" width="40.875" customWidth="1"/>
     <col min="8" max="8" width="14.625" customWidth="1"/>
@@ -2240,7 +2249,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="48.75">
+    <row r="32" spans="1:10" ht="18.75" customHeight="1">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -2272,7 +2281,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="32.25">
+    <row r="33" spans="1:10" ht="17.25" customHeight="1">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -2336,7 +2345,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="21" customHeight="1">
+    <row r="35" spans="1:10" ht="15" customHeight="1">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -2368,7 +2377,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="16.5">
+    <row r="36" spans="1:10" ht="15" customHeight="1">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -2378,29 +2387,29 @@
       <c r="C36" t="s">
         <v>104</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E36" t="s">
+        <v>104</v>
+      </c>
+      <c r="F36" t="s">
+        <v>102</v>
+      </c>
+      <c r="G36" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E36" t="s">
-        <v>106</v>
-      </c>
-      <c r="F36" t="s">
-        <v>107</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="H36" t="s">
-        <v>109</v>
+      <c r="H36">
+        <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>109</v>
+        <v>15</v>
       </c>
       <c r="J36" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="16.5">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="15" customHeight="1">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -2408,31 +2417,31 @@
         <v>11</v>
       </c>
       <c r="C37" t="s">
-        <v>110</v>
-      </c>
-      <c r="D37" t="s">
-        <v>105</v>
+        <v>106</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="E37" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F37" t="s">
+        <v>102</v>
+      </c>
+      <c r="G37" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G37" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="H37" t="s">
-        <v>109</v>
+      <c r="H37">
+        <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>109</v>
+        <v>15</v>
       </c>
       <c r="J37" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="20.25" customHeight="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="16.5">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -2440,31 +2449,31 @@
         <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D38" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E38" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F38" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="H38" t="s">
-        <v>109</v>
+        <v>112</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>109</v>
+        <v>15</v>
       </c>
       <c r="J38" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="21.75" customHeight="1">
+    <row r="39" spans="1:10" ht="16.5">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -2472,19 +2481,19 @@
         <v>11</v>
       </c>
       <c r="C39" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D39" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="E39" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F39" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -2496,24 +2505,28 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.75">
+    <row r="40" spans="1:10" ht="20.25" customHeight="1">
       <c r="A40" t="s">
         <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>12</v>
+        <v>116</v>
       </c>
       <c r="D40" t="s">
-        <v>13</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
+        <v>109</v>
+      </c>
+      <c r="E40" t="s">
+        <v>117</v>
+      </c>
+      <c r="F40" t="s">
+        <v>111</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="H40">
         <v>0</v>
       </c>
@@ -2521,27 +2534,31 @@
         <v>15</v>
       </c>
       <c r="J40" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="15.75">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="21.75" customHeight="1">
       <c r="A41" t="s">
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="C41" t="s">
-        <v>17</v>
+        <v>119</v>
       </c>
       <c r="D41" t="s">
-        <v>13</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
+        <v>92</v>
+      </c>
+      <c r="E41" t="s">
+        <v>120</v>
+      </c>
+      <c r="F41" t="s">
+        <v>94</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="H41">
         <v>0</v>
       </c>
@@ -2549,10 +2566,10 @@
         <v>15</v>
       </c>
       <c r="J41" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="15.75">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="21.75" customHeight="1">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -2560,13 +2577,19 @@
         <v>61</v>
       </c>
       <c r="C42" t="s">
-        <v>19</v>
+        <v>119</v>
       </c>
       <c r="D42" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="E42" t="s">
-        <v>21</v>
+        <v>120</v>
+      </c>
+      <c r="F42" t="s">
+        <v>122</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="H42">
         <v>0</v>
@@ -2575,7 +2598,7 @@
         <v>15</v>
       </c>
       <c r="J42" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="15.75">
@@ -2586,14 +2609,16 @@
         <v>61</v>
       </c>
       <c r="C43" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D43" t="s">
-        <v>20</v>
-      </c>
-      <c r="E43" t="s">
-        <v>24</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
       <c r="H43">
         <v>0</v>
       </c>
@@ -2601,7 +2626,7 @@
         <v>15</v>
       </c>
       <c r="J43" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15.75">
@@ -2612,14 +2637,16 @@
         <v>61</v>
       </c>
       <c r="C44" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D44" t="s">
-        <v>20</v>
-      </c>
-      <c r="E44" t="s">
-        <v>26</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
       <c r="H44">
         <v>0</v>
       </c>
@@ -2627,7 +2654,7 @@
         <v>15</v>
       </c>
       <c r="J44" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15.75">
@@ -2638,13 +2665,13 @@
         <v>61</v>
       </c>
       <c r="C45" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="D45" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="E45" t="s">
-        <v>78</v>
+        <v>21</v>
       </c>
       <c r="H45">
         <v>0</v>
@@ -2664,13 +2691,13 @@
         <v>61</v>
       </c>
       <c r="C46" t="s">
-        <v>79</v>
+        <v>23</v>
       </c>
       <c r="D46" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="E46" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="H46">
         <v>0</v>
@@ -2690,13 +2717,13 @@
         <v>61</v>
       </c>
       <c r="C47" t="s">
-        <v>81</v>
+        <v>25</v>
       </c>
       <c r="D47" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="E47" t="s">
-        <v>82</v>
+        <v>26</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -2716,13 +2743,13 @@
         <v>61</v>
       </c>
       <c r="C48" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D48" t="s">
         <v>77</v>
       </c>
       <c r="E48" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H48">
         <v>0</v>
@@ -2742,13 +2769,13 @@
         <v>61</v>
       </c>
       <c r="C49" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="D49" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="E49" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="H49">
         <v>0</v>
@@ -2757,7 +2784,7 @@
         <v>15</v>
       </c>
       <c r="J49" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="15.75">
@@ -2768,13 +2795,13 @@
         <v>61</v>
       </c>
       <c r="C50" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="D50" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="E50" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="H50">
         <v>0</v>
@@ -2783,7 +2810,7 @@
         <v>15</v>
       </c>
       <c r="J50" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="15.75">
@@ -2794,45 +2821,39 @@
         <v>61</v>
       </c>
       <c r="C51" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="D51" t="s">
+        <v>77</v>
+      </c>
+      <c r="E51" t="s">
+        <v>84</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51" t="s">
+        <v>15</v>
+      </c>
+      <c r="J51" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="15.75">
+      <c r="A52" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" t="s">
+        <v>61</v>
+      </c>
+      <c r="C52" t="s">
+        <v>66</v>
+      </c>
+      <c r="D52" t="s">
         <v>67</v>
       </c>
-      <c r="E51" t="s">
-        <v>72</v>
-      </c>
-      <c r="H51">
-        <v>0</v>
-      </c>
-      <c r="I51" t="s">
-        <v>15</v>
-      </c>
-      <c r="J51" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="15" customHeight="1">
-      <c r="A52" t="s">
-        <v>10</v>
-      </c>
-      <c r="B52" t="s">
-        <v>61</v>
-      </c>
-      <c r="C52" t="s">
-        <v>116</v>
-      </c>
-      <c r="D52" t="s">
-        <v>92</v>
-      </c>
       <c r="E52" t="s">
-        <v>117</v>
-      </c>
-      <c r="F52" t="s">
-        <v>119</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="H52">
         <v>0</v>
@@ -2844,7 +2865,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="16.5">
+    <row r="53" spans="1:10" ht="15.75">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -2852,31 +2873,25 @@
         <v>61</v>
       </c>
       <c r="C53" t="s">
-        <v>104</v>
+        <v>69</v>
       </c>
       <c r="D53" t="s">
-        <v>105</v>
+        <v>67</v>
       </c>
       <c r="E53" t="s">
-        <v>106</v>
-      </c>
-      <c r="F53" t="s">
-        <v>120</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="H53" t="s">
-        <v>109</v>
+        <v>70</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
       </c>
       <c r="I53" t="s">
-        <v>109</v>
+        <v>15</v>
       </c>
       <c r="J53" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="16.5">
+    <row r="54" spans="1:10" ht="15.75">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -2884,31 +2899,25 @@
         <v>61</v>
       </c>
       <c r="C54" t="s">
-        <v>110</v>
+        <v>71</v>
       </c>
       <c r="D54" t="s">
-        <v>105</v>
+        <v>67</v>
       </c>
       <c r="E54" t="s">
-        <v>111</v>
-      </c>
-      <c r="F54" t="s">
-        <v>120</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="H54" t="s">
-        <v>109</v>
+        <v>72</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
       </c>
       <c r="I54" t="s">
-        <v>109</v>
+        <v>15</v>
       </c>
       <c r="J54" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="20.25" customHeight="1">
+    <row r="55" spans="1:10" ht="15" customHeight="1">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -2916,31 +2925,31 @@
         <v>61</v>
       </c>
       <c r="C55" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="D55" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="E55" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="F55" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="H55" t="s">
-        <v>109</v>
+        <v>121</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
       </c>
       <c r="I55" t="s">
-        <v>109</v>
+        <v>15</v>
       </c>
       <c r="J55" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="15.75">
+    <row r="56" spans="1:10" ht="16.5">
       <c r="A56" t="s">
         <v>10</v>
       </c>
@@ -2948,19 +2957,19 @@
         <v>61</v>
       </c>
       <c r="C56" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="D56" t="s">
-        <v>13</v>
+        <v>109</v>
       </c>
       <c r="E56" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F56" t="s">
-        <v>119</v>
-      </c>
-      <c r="G56" t="s">
-        <v>122</v>
+        <v>123</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="H56">
         <v>0</v>
@@ -2972,7 +2981,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="15.75">
+    <row r="57" spans="1:10" ht="16.5">
       <c r="A57" t="s">
         <v>10</v>
       </c>
@@ -2980,54 +2989,60 @@
         <v>61</v>
       </c>
       <c r="C57" t="s">
+        <v>113</v>
+      </c>
+      <c r="D57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F57" t="s">
         <v>123</v>
       </c>
-      <c r="D57" t="s">
-        <v>13</v>
-      </c>
-      <c r="E57" t="s">
+      <c r="G57" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57" t="s">
+        <v>15</v>
+      </c>
+      <c r="J57" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="20.25" customHeight="1">
+      <c r="A58" t="s">
+        <v>10</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58" t="s">
+        <v>116</v>
+      </c>
+      <c r="D58" t="s">
+        <v>109</v>
+      </c>
+      <c r="E58" t="s">
+        <v>117</v>
+      </c>
+      <c r="F58" t="s">
         <v>123</v>
       </c>
-      <c r="F57" t="s">
-        <v>119</v>
-      </c>
-      <c r="G57" t="s">
-        <v>124</v>
-      </c>
-      <c r="H57">
-        <v>0</v>
-      </c>
-      <c r="I57" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="15.75">
-      <c r="A58" t="s">
-        <v>10</v>
-      </c>
-      <c r="B58" t="s">
-        <v>61</v>
-      </c>
-      <c r="C58" t="s">
-        <v>125</v>
-      </c>
-      <c r="D58" t="s">
-        <v>13</v>
-      </c>
-      <c r="E58" t="s">
-        <v>125</v>
-      </c>
-      <c r="F58" t="s">
-        <v>119</v>
-      </c>
-      <c r="G58" t="s">
-        <v>126</v>
+      <c r="G58" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="H58">
         <v>0</v>
       </c>
       <c r="I58" t="s">
         <v>15</v>
+      </c>
+      <c r="J58" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="15.75">
@@ -3038,19 +3053,19 @@
         <v>61</v>
       </c>
       <c r="C59" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D59" t="s">
         <v>13</v>
       </c>
       <c r="E59" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F59" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="G59" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -3058,8 +3073,11 @@
       <c r="I59" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" ht="16.5" customHeight="1">
+      <c r="J59" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="15.75">
       <c r="A60" t="s">
         <v>10</v>
       </c>
@@ -3067,19 +3085,19 @@
         <v>61</v>
       </c>
       <c r="C60" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D60" t="s">
         <v>13</v>
       </c>
       <c r="E60" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F60" t="s">
-        <v>119</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>130</v>
+        <v>122</v>
+      </c>
+      <c r="G60" t="s">
+        <v>127</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -3088,7 +3106,7 @@
         <v>15</v>
       </c>
       <c r="J60" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="15.75">
@@ -3099,28 +3117,28 @@
         <v>61</v>
       </c>
       <c r="C61" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D61" t="s">
-        <v>132</v>
+        <v>13</v>
       </c>
       <c r="E61" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F61" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="G61" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="H61">
         <v>0</v>
       </c>
       <c r="I61" t="s">
-        <v>109</v>
+        <v>15</v>
       </c>
       <c r="J61" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="15.75">
@@ -3131,19 +3149,19 @@
         <v>61</v>
       </c>
       <c r="C62" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D62" t="s">
-        <v>136</v>
+        <v>13</v>
       </c>
       <c r="E62" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F62" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="G62" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="H62">
         <v>0</v>
@@ -3152,10 +3170,10 @@
         <v>15</v>
       </c>
       <c r="J62" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="21.75" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="16.5" customHeight="1">
       <c r="A63" t="s">
         <v>10</v>
       </c>
@@ -3163,31 +3181,31 @@
         <v>61</v>
       </c>
       <c r="C63" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="D63" t="s">
-        <v>140</v>
+        <v>13</v>
       </c>
       <c r="E63" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="F63" t="s">
-        <v>141</v>
-      </c>
-      <c r="G63" s="3" t="s">
-        <v>142</v>
+        <v>122</v>
+      </c>
+      <c r="G63" t="s">
+        <v>133</v>
       </c>
       <c r="H63">
         <v>0</v>
       </c>
       <c r="I63" t="s">
-        <v>109</v>
+        <v>15</v>
       </c>
       <c r="J63" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="48.75">
+    <row r="64" spans="1:10" ht="15.75">
       <c r="A64" t="s">
         <v>10</v>
       </c>
@@ -3195,19 +3213,19 @@
         <v>61</v>
       </c>
       <c r="C64" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="D64" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="E64" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="F64" t="s">
-        <v>146</v>
-      </c>
-      <c r="G64" s="3" t="s">
-        <v>147</v>
+        <v>136</v>
+      </c>
+      <c r="G64" t="s">
+        <v>137</v>
       </c>
       <c r="H64">
         <v>0</v>
@@ -3219,7 +3237,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="32.25">
+    <row r="65" spans="1:11" ht="15.75">
       <c r="A65" t="s">
         <v>10</v>
       </c>
@@ -3227,19 +3245,19 @@
         <v>61</v>
       </c>
       <c r="C65" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="D65" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="E65" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="F65" t="s">
-        <v>150</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>151</v>
+        <v>140</v>
+      </c>
+      <c r="G65" t="s">
+        <v>141</v>
       </c>
       <c r="H65">
         <v>0</v>
@@ -3248,10 +3266,10 @@
         <v>15</v>
       </c>
       <c r="J65" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" ht="32.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="21.75" customHeight="1">
       <c r="A66" t="s">
         <v>10</v>
       </c>
@@ -3259,19 +3277,19 @@
         <v>61</v>
       </c>
       <c r="C66" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="D66" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="E66" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="F66" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="H66">
         <v>0</v>
@@ -3291,19 +3309,19 @@
         <v>61</v>
       </c>
       <c r="C67" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D67" t="s">
+        <v>147</v>
+      </c>
+      <c r="E67" t="s">
+        <v>148</v>
+      </c>
+      <c r="F67" t="s">
         <v>149</v>
       </c>
-      <c r="E67" t="s">
-        <v>154</v>
-      </c>
-      <c r="F67" t="s">
+      <c r="G67" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="G67" s="3" t="s">
-        <v>155</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -3323,19 +3341,19 @@
         <v>61</v>
       </c>
       <c r="C68" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D68" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E68" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F68" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H68">
         <v>0</v>
@@ -3347,7 +3365,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="48.75">
+    <row r="69" spans="1:11" ht="32.25">
       <c r="A69" t="s">
         <v>10</v>
       </c>
@@ -3355,19 +3373,19 @@
         <v>61</v>
       </c>
       <c r="C69" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D69" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E69" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F69" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="H69">
         <v>0</v>
@@ -3378,11 +3396,8 @@
       <c r="J69" t="s">
         <v>65</v>
       </c>
-      <c r="K69" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" ht="64.5">
+    </row>
+    <row r="70" spans="1:11" ht="48.75">
       <c r="A70" t="s">
         <v>10</v>
       </c>
@@ -3390,19 +3405,19 @@
         <v>61</v>
       </c>
       <c r="C70" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D70" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E70" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="F70" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="H70">
         <v>0</v>
@@ -3422,19 +3437,19 @@
         <v>61</v>
       </c>
       <c r="C71" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D71" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E71" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F71" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="H71">
         <v>0</v>
@@ -3446,7 +3461,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="15.75">
+    <row r="72" spans="1:11" ht="48.75">
       <c r="A72" t="s">
         <v>10</v>
       </c>
@@ -3454,13 +3469,19 @@
         <v>61</v>
       </c>
       <c r="C72" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D72" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="E72" t="s">
-        <v>168</v>
+        <v>161</v>
+      </c>
+      <c r="F72" t="s">
+        <v>162</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>163</v>
       </c>
       <c r="H72">
         <v>0</v>
@@ -3471,8 +3492,11 @@
       <c r="J72" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" ht="15.75">
+      <c r="K72" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="64.5">
       <c r="A73" t="s">
         <v>10</v>
       </c>
@@ -3480,13 +3504,19 @@
         <v>61</v>
       </c>
       <c r="C73" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D73" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="E73" t="s">
-        <v>171</v>
+        <v>165</v>
+      </c>
+      <c r="F73" t="s">
+        <v>162</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>166</v>
       </c>
       <c r="H73">
         <v>0</v>
@@ -3495,10 +3525,10 @@
         <v>15</v>
       </c>
       <c r="J73" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" ht="15.75">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="32.25">
       <c r="A74" t="s">
         <v>10</v>
       </c>
@@ -3506,13 +3536,19 @@
         <v>61</v>
       </c>
       <c r="C74" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D74" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="E74" t="s">
-        <v>72</v>
+        <v>167</v>
+      </c>
+      <c r="F74" t="s">
+        <v>162</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>168</v>
       </c>
       <c r="H74">
         <v>0</v>
@@ -3524,7 +3560,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="32.25">
+    <row r="75" spans="1:11" ht="15.75">
       <c r="A75" t="s">
         <v>10</v>
       </c>
@@ -3532,19 +3568,13 @@
         <v>61</v>
       </c>
       <c r="C75" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D75" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E75" t="s">
-        <v>174</v>
-      </c>
-      <c r="F75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G75" s="3" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="H75">
         <v>0</v>
@@ -3553,7 +3583,7 @@
         <v>15</v>
       </c>
       <c r="J75" t="s">
-        <v>96</v>
+        <v>65</v>
       </c>
     </row>
     <row r="76" spans="1:11" ht="15.75">
@@ -3564,13 +3594,13 @@
         <v>61</v>
       </c>
       <c r="C76" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D76" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E76" t="s">
-        <v>72</v>
+        <v>174</v>
       </c>
       <c r="H76">
         <v>0</v>
@@ -3579,7 +3609,7 @@
         <v>15</v>
       </c>
       <c r="J76" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
     </row>
     <row r="77" spans="1:11" ht="15.75">
@@ -3590,13 +3620,13 @@
         <v>61</v>
       </c>
       <c r="C77" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D77" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E77" t="s">
-        <v>182</v>
+        <v>72</v>
       </c>
       <c r="H77">
         <v>0</v>
@@ -3605,7 +3635,7 @@
         <v>15</v>
       </c>
       <c r="J77" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
     </row>
     <row r="78" spans="1:11" ht="32.25">
@@ -3616,19 +3646,19 @@
         <v>61</v>
       </c>
       <c r="C78" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D78" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="E78" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="F78" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="H78">
         <v>0</v>
@@ -3637,7 +3667,7 @@
         <v>15</v>
       </c>
       <c r="J78" t="s">
-        <v>22</v>
+        <v>96</v>
       </c>
     </row>
     <row r="79" spans="1:11" ht="15.75">
@@ -3648,13 +3678,13 @@
         <v>61</v>
       </c>
       <c r="C79" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D79" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="E79" t="s">
-        <v>189</v>
+        <v>72</v>
       </c>
       <c r="H79">
         <v>0</v>
@@ -3674,39 +3704,45 @@
         <v>61</v>
       </c>
       <c r="C80" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="D80" t="s">
+        <v>184</v>
+      </c>
+      <c r="E80" t="s">
+        <v>185</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+      <c r="I80" t="s">
+        <v>15</v>
+      </c>
+      <c r="J80" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="32.25">
+      <c r="A81" t="s">
+        <v>10</v>
+      </c>
+      <c r="B81" t="s">
+        <v>61</v>
+      </c>
+      <c r="C81" t="s">
+        <v>186</v>
+      </c>
+      <c r="D81" t="s">
+        <v>187</v>
+      </c>
+      <c r="E81" t="s">
+        <v>186</v>
+      </c>
+      <c r="F81" t="s">
         <v>188</v>
       </c>
-      <c r="E80" t="s">
-        <v>191</v>
-      </c>
-      <c r="H80">
-        <v>0</v>
-      </c>
-      <c r="I80" t="s">
-        <v>15</v>
-      </c>
-      <c r="J80" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="15.75">
-      <c r="A81" t="s">
-        <v>10</v>
-      </c>
-      <c r="B81" t="s">
-        <v>61</v>
-      </c>
-      <c r="C81" t="s">
-        <v>192</v>
-      </c>
-      <c r="D81" t="s">
-        <v>188</v>
-      </c>
-      <c r="E81" t="s">
-        <v>193</v>
+      <c r="G81" s="3" t="s">
+        <v>189</v>
       </c>
       <c r="H81">
         <v>0</v>
@@ -3715,7 +3751,7 @@
         <v>15</v>
       </c>
       <c r="J81" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="15.75">
@@ -3726,13 +3762,13 @@
         <v>61</v>
       </c>
       <c r="C82" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D82" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E82" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H82">
         <v>0</v>
@@ -3752,13 +3788,13 @@
         <v>61</v>
       </c>
       <c r="C83" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D83" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E83" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H83">
         <v>0</v>
@@ -3778,13 +3814,13 @@
         <v>61</v>
       </c>
       <c r="C84" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D84" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E84" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H84">
         <v>0</v>
@@ -3804,13 +3840,13 @@
         <v>61</v>
       </c>
       <c r="C85" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D85" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E85" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H85">
         <v>0</v>
@@ -3830,13 +3866,13 @@
         <v>61</v>
       </c>
       <c r="C86" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D86" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E86" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H86">
         <v>0</v>
@@ -3856,13 +3892,13 @@
         <v>61</v>
       </c>
       <c r="C87" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D87" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E87" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="H87">
         <v>0</v>
@@ -3882,13 +3918,13 @@
         <v>61</v>
       </c>
       <c r="C88" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D88" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E88" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="H88">
         <v>0</v>
@@ -3908,13 +3944,13 @@
         <v>61</v>
       </c>
       <c r="C89" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D89" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="E89" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="H89">
         <v>0</v>
@@ -3923,7 +3959,7 @@
         <v>15</v>
       </c>
       <c r="J89" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="15.75">
@@ -3934,45 +3970,39 @@
         <v>61</v>
       </c>
       <c r="C90" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D90" t="s">
+        <v>191</v>
+      </c>
+      <c r="E90" t="s">
+        <v>208</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+      <c r="I90" t="s">
+        <v>15</v>
+      </c>
+      <c r="J90" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" ht="15.75">
+      <c r="A91" t="s">
+        <v>10</v>
+      </c>
+      <c r="B91" t="s">
+        <v>61</v>
+      </c>
+      <c r="C91" t="s">
         <v>209</v>
       </c>
-      <c r="E90" t="s">
-        <v>212</v>
-      </c>
-      <c r="H90">
-        <v>0</v>
-      </c>
-      <c r="I90" t="s">
-        <v>15</v>
-      </c>
-      <c r="J90" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" ht="32.25">
-      <c r="A91" t="s">
-        <v>10</v>
-      </c>
-      <c r="B91" t="s">
-        <v>61</v>
-      </c>
-      <c r="C91" t="s">
-        <v>213</v>
-      </c>
       <c r="D91" t="s">
-        <v>214</v>
+        <v>191</v>
       </c>
       <c r="E91" t="s">
-        <v>213</v>
-      </c>
-      <c r="F91" t="s">
-        <v>215</v>
-      </c>
-      <c r="G91" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="H91">
         <v>0</v>
@@ -3981,7 +4011,7 @@
         <v>15</v>
       </c>
       <c r="J91" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="15.75">
@@ -3992,19 +4022,13 @@
         <v>61</v>
       </c>
       <c r="C92" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E92" t="s">
-        <v>217</v>
-      </c>
-      <c r="F92" t="s">
-        <v>219</v>
-      </c>
-      <c r="G92" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="H92">
         <v>0</v>
@@ -4024,19 +4048,13 @@
         <v>61</v>
       </c>
       <c r="C93" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D93" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E93" t="s">
-        <v>221</v>
-      </c>
-      <c r="F93" t="s">
-        <v>219</v>
-      </c>
-      <c r="G93" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="H93">
         <v>0</v>
@@ -4048,7 +4066,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="15.75">
+    <row r="94" spans="1:10" ht="32.25">
       <c r="A94" t="s">
         <v>10</v>
       </c>
@@ -4056,20 +4074,20 @@
         <v>61</v>
       </c>
       <c r="C94" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="D94" t="s">
+        <v>217</v>
+      </c>
+      <c r="E94" t="s">
+        <v>216</v>
+      </c>
+      <c r="F94" t="s">
         <v>218</v>
       </c>
-      <c r="E94" t="s">
-        <v>223</v>
-      </c>
-      <c r="F94" t="s">
+      <c r="G94" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="G94" t="s">
-        <v>224</v>
-      </c>
       <c r="H94">
         <v>0</v>
       </c>
@@ -4077,7 +4095,7 @@
         <v>15</v>
       </c>
       <c r="J94" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
     </row>
     <row r="95" spans="1:10" ht="15.75">
@@ -4088,19 +4106,19 @@
         <v>61</v>
       </c>
       <c r="C95" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D95" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="E95" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F95" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="G95" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="H95">
         <v>0</v>
@@ -4120,13 +4138,19 @@
         <v>61</v>
       </c>
       <c r="C96" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D96" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="E96" t="s">
-        <v>72</v>
+        <v>224</v>
+      </c>
+      <c r="F96" t="s">
+        <v>222</v>
+      </c>
+      <c r="G96" t="s">
+        <v>225</v>
       </c>
       <c r="H96">
         <v>0</v>
@@ -4135,7 +4159,7 @@
         <v>15</v>
       </c>
       <c r="J96" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
     </row>
     <row r="97" spans="1:10" ht="15.75">
@@ -4146,13 +4170,19 @@
         <v>61</v>
       </c>
       <c r="C97" t="s">
-        <v>27</v>
+        <v>226</v>
       </c>
       <c r="D97" t="s">
-        <v>28</v>
+        <v>221</v>
       </c>
       <c r="E97" t="s">
-        <v>29</v>
+        <v>226</v>
+      </c>
+      <c r="F97" t="s">
+        <v>222</v>
+      </c>
+      <c r="G97" t="s">
+        <v>227</v>
       </c>
       <c r="H97">
         <v>0</v>
@@ -4161,7 +4191,7 @@
         <v>15</v>
       </c>
       <c r="J97" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="98" spans="1:10" ht="15.75">
@@ -4172,13 +4202,19 @@
         <v>61</v>
       </c>
       <c r="C98" t="s">
-        <v>31</v>
+        <v>228</v>
       </c>
       <c r="D98" t="s">
-        <v>28</v>
+        <v>221</v>
       </c>
       <c r="E98" t="s">
-        <v>32</v>
+        <v>228</v>
+      </c>
+      <c r="F98" t="s">
+        <v>222</v>
+      </c>
+      <c r="G98" t="s">
+        <v>229</v>
       </c>
       <c r="H98">
         <v>0</v>
@@ -4187,7 +4223,7 @@
         <v>15</v>
       </c>
       <c r="J98" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="99" spans="1:10" ht="15.75">
@@ -4198,13 +4234,13 @@
         <v>61</v>
       </c>
       <c r="C99" t="s">
-        <v>33</v>
+        <v>230</v>
       </c>
       <c r="D99" t="s">
-        <v>28</v>
+        <v>231</v>
       </c>
       <c r="E99" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="H99">
         <v>0</v>
@@ -4213,7 +4249,7 @@
         <v>15</v>
       </c>
       <c r="J99" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
     </row>
     <row r="100" spans="1:10" ht="15.75">
@@ -4224,13 +4260,13 @@
         <v>61</v>
       </c>
       <c r="C100" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D100" t="s">
         <v>28</v>
       </c>
       <c r="E100" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="H100">
         <v>0</v>
@@ -4250,13 +4286,13 @@
         <v>61</v>
       </c>
       <c r="C101" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D101" t="s">
         <v>28</v>
       </c>
       <c r="E101" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H101">
         <v>0</v>
@@ -4276,13 +4312,13 @@
         <v>61</v>
       </c>
       <c r="C102" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D102" t="s">
         <v>28</v>
       </c>
       <c r="E102" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H102">
         <v>0</v>
@@ -4302,13 +4338,13 @@
         <v>61</v>
       </c>
       <c r="C103" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D103" t="s">
         <v>28</v>
       </c>
       <c r="E103" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H103">
         <v>0</v>
@@ -4328,13 +4364,13 @@
         <v>61</v>
       </c>
       <c r="C104" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D104" t="s">
         <v>28</v>
       </c>
       <c r="E104" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H104">
         <v>0</v>
@@ -4354,13 +4390,13 @@
         <v>61</v>
       </c>
       <c r="C105" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D105" t="s">
         <v>28</v>
       </c>
       <c r="E105" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="H105">
         <v>0</v>
@@ -4380,13 +4416,13 @@
         <v>61</v>
       </c>
       <c r="C106" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D106" t="s">
         <v>28</v>
       </c>
       <c r="E106" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H106">
         <v>0</v>
@@ -4406,13 +4442,13 @@
         <v>61</v>
       </c>
       <c r="C107" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D107" t="s">
         <v>28</v>
       </c>
       <c r="E107" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H107">
         <v>0</v>
@@ -4432,13 +4468,13 @@
         <v>61</v>
       </c>
       <c r="C108" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D108" t="s">
         <v>28</v>
       </c>
       <c r="E108" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H108">
         <v>0</v>
@@ -4458,13 +4494,13 @@
         <v>61</v>
       </c>
       <c r="C109" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D109" t="s">
         <v>28</v>
       </c>
       <c r="E109" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H109">
         <v>0</v>
@@ -4484,13 +4520,13 @@
         <v>61</v>
       </c>
       <c r="C110" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D110" t="s">
         <v>28</v>
       </c>
       <c r="E110" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="H110">
         <v>0</v>
@@ -4510,13 +4546,13 @@
         <v>61</v>
       </c>
       <c r="C111" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D111" t="s">
         <v>28</v>
       </c>
       <c r="E111" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="H111">
         <v>0</v>
@@ -4536,13 +4572,13 @@
         <v>61</v>
       </c>
       <c r="C112" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D112" t="s">
         <v>28</v>
       </c>
       <c r="E112" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="H112">
         <v>0</v>
@@ -4562,199 +4598,187 @@
         <v>61</v>
       </c>
       <c r="C113" t="s">
-        <v>229</v>
+        <v>55</v>
       </c>
       <c r="D113" t="s">
-        <v>230</v>
+        <v>28</v>
       </c>
       <c r="E113" t="s">
+        <v>56</v>
+      </c>
+      <c r="H113">
+        <v>0</v>
+      </c>
+      <c r="I113" t="s">
+        <v>15</v>
+      </c>
+      <c r="J113" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" ht="15.75">
+      <c r="A114" t="s">
+        <v>10</v>
+      </c>
+      <c r="B114" t="s">
+        <v>61</v>
+      </c>
+      <c r="C114" t="s">
+        <v>57</v>
+      </c>
+      <c r="D114" t="s">
+        <v>28</v>
+      </c>
+      <c r="E114" t="s">
+        <v>58</v>
+      </c>
+      <c r="H114">
+        <v>0</v>
+      </c>
+      <c r="I114" t="s">
+        <v>15</v>
+      </c>
+      <c r="J114" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" ht="15.75">
+      <c r="A115" t="s">
+        <v>10</v>
+      </c>
+      <c r="B115" t="s">
+        <v>61</v>
+      </c>
+      <c r="C115" t="s">
+        <v>59</v>
+      </c>
+      <c r="D115" t="s">
+        <v>28</v>
+      </c>
+      <c r="E115" t="s">
+        <v>60</v>
+      </c>
+      <c r="H115">
+        <v>0</v>
+      </c>
+      <c r="I115" t="s">
+        <v>15</v>
+      </c>
+      <c r="J115" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" ht="15.75">
+      <c r="A116" t="s">
+        <v>10</v>
+      </c>
+      <c r="B116" t="s">
+        <v>61</v>
+      </c>
+      <c r="C116" t="s">
+        <v>232</v>
+      </c>
+      <c r="D116" t="s">
+        <v>233</v>
+      </c>
+      <c r="E116" t="s">
         <v>72</v>
       </c>
-      <c r="H113">
-        <v>0</v>
-      </c>
-      <c r="I113" t="s">
-        <v>15</v>
-      </c>
-      <c r="J113" t="s">
+      <c r="H116">
+        <v>0</v>
+      </c>
+      <c r="I116" t="s">
+        <v>15</v>
+      </c>
+      <c r="J116" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="15" customHeight="1">
-      <c r="A114" t="s">
-        <v>10</v>
-      </c>
-      <c r="B114" t="s">
-        <v>61</v>
-      </c>
-      <c r="C114" t="s">
+    <row r="117" spans="1:10" ht="15" customHeight="1">
+      <c r="A117" t="s">
+        <v>10</v>
+      </c>
+      <c r="B117" t="s">
+        <v>61</v>
+      </c>
+      <c r="C117" t="s">
         <v>100</v>
       </c>
-      <c r="D114" s="3" t="s">
+      <c r="D117" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E114" t="s">
+      <c r="E117" t="s">
         <v>100</v>
       </c>
-      <c r="F114" t="s">
-        <v>231</v>
-      </c>
-      <c r="G114" s="3" t="s">
+      <c r="F117" t="s">
+        <v>234</v>
+      </c>
+      <c r="G117" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="H114">
-        <v>0</v>
-      </c>
-      <c r="I114" t="s">
-        <v>15</v>
-      </c>
-      <c r="J114" t="s">
+      <c r="H117">
+        <v>0</v>
+      </c>
+      <c r="I117" t="s">
+        <v>15</v>
+      </c>
+      <c r="J117" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A115" t="s">
-        <v>10</v>
-      </c>
-      <c r="B115" t="s">
-        <v>61</v>
-      </c>
-      <c r="C115" t="s">
-        <v>91</v>
-      </c>
-      <c r="D115" t="s">
-        <v>92</v>
-      </c>
-      <c r="E115" t="s">
-        <v>93</v>
-      </c>
-      <c r="F115" t="s">
-        <v>232</v>
-      </c>
-      <c r="G115" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="H115">
-        <v>0</v>
-      </c>
-      <c r="I115" t="s">
-        <v>15</v>
-      </c>
-      <c r="J115" t="s">
+    <row r="118" spans="1:10" ht="15" customHeight="1">
+      <c r="A118" t="s">
+        <v>10</v>
+      </c>
+      <c r="B118" t="s">
+        <v>61</v>
+      </c>
+      <c r="C118" t="s">
+        <v>104</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E118" t="s">
+        <v>104</v>
+      </c>
+      <c r="F118" t="s">
+        <v>234</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H118">
+        <v>0</v>
+      </c>
+      <c r="I118" t="s">
+        <v>15</v>
+      </c>
+      <c r="J118" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="116" spans="1:10" ht="15" customHeight="1">
-      <c r="A116" t="s">
-        <v>10</v>
-      </c>
-      <c r="B116" t="s">
-        <v>61</v>
-      </c>
-      <c r="C116" t="s">
-        <v>97</v>
-      </c>
-      <c r="D116" t="s">
-        <v>92</v>
-      </c>
-      <c r="E116" t="s">
-        <v>98</v>
-      </c>
-      <c r="F116" t="s">
-        <v>232</v>
-      </c>
-      <c r="G116" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="H116">
-        <v>0</v>
-      </c>
-      <c r="I116" t="s">
-        <v>15</v>
-      </c>
-      <c r="J116" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10" ht="15.75">
-      <c r="A117" t="s">
-        <v>233</v>
-      </c>
-      <c r="B117" t="s">
-        <v>11</v>
-      </c>
-      <c r="C117" t="s">
+    <row r="119" spans="1:10" ht="15" customHeight="1">
+      <c r="A119" t="s">
+        <v>10</v>
+      </c>
+      <c r="B119" t="s">
+        <v>61</v>
+      </c>
+      <c r="C119" t="s">
+        <v>106</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E119" t="s">
+        <v>106</v>
+      </c>
+      <c r="F119" t="s">
         <v>234</v>
       </c>
-      <c r="D117" t="s">
-        <v>235</v>
-      </c>
-      <c r="E117" t="s">
-        <v>236</v>
-      </c>
-      <c r="H117">
-        <v>0</v>
-      </c>
-      <c r="I117" t="s">
-        <v>15</v>
-      </c>
-      <c r="J117" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10" ht="15.75">
-      <c r="A118" t="s">
-        <v>233</v>
-      </c>
-      <c r="B118" t="s">
-        <v>11</v>
-      </c>
-      <c r="C118" t="s">
-        <v>237</v>
-      </c>
-      <c r="D118" t="s">
-        <v>238</v>
-      </c>
-      <c r="E118" t="s">
-        <v>239</v>
-      </c>
-      <c r="F118" t="s">
-        <v>240</v>
-      </c>
-      <c r="G118" t="s">
-        <v>241</v>
-      </c>
-      <c r="H118">
-        <v>0</v>
-      </c>
-      <c r="I118" t="s">
-        <v>15</v>
-      </c>
-      <c r="J118" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10" ht="15.75">
-      <c r="A119" t="s">
-        <v>233</v>
-      </c>
-      <c r="B119" t="s">
-        <v>11</v>
-      </c>
-      <c r="C119" t="s">
-        <v>242</v>
-      </c>
-      <c r="D119" t="s">
-        <v>243</v>
-      </c>
-      <c r="E119" t="s">
-        <v>244</v>
-      </c>
-      <c r="F119" t="s">
-        <v>245</v>
-      </c>
-      <c r="G119" t="s">
-        <v>246</v>
+      <c r="G119" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="H119">
         <v>0</v>
@@ -4766,27 +4790,27 @@
         <v>96</v>
       </c>
     </row>
-    <row r="120" spans="1:10" ht="15.75">
+    <row r="120" spans="1:10" ht="15.75" customHeight="1">
       <c r="A120" t="s">
-        <v>233</v>
+        <v>10</v>
       </c>
       <c r="B120" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="C120" t="s">
-        <v>247</v>
+        <v>91</v>
       </c>
       <c r="D120" t="s">
-        <v>243</v>
+        <v>92</v>
       </c>
       <c r="E120" t="s">
-        <v>248</v>
+        <v>93</v>
       </c>
       <c r="F120" t="s">
-        <v>245</v>
-      </c>
-      <c r="G120" t="s">
-        <v>249</v>
+        <v>235</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="H120">
         <v>0</v>
@@ -4798,27 +4822,27 @@
         <v>96</v>
       </c>
     </row>
-    <row r="121" spans="1:10" ht="15.75">
+    <row r="121" spans="1:10" ht="15" customHeight="1">
       <c r="A121" t="s">
-        <v>233</v>
+        <v>10</v>
       </c>
       <c r="B121" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="C121" t="s">
-        <v>250</v>
+        <v>97</v>
       </c>
       <c r="D121" t="s">
-        <v>243</v>
+        <v>92</v>
       </c>
       <c r="E121" t="s">
-        <v>251</v>
+        <v>98</v>
       </c>
       <c r="F121" t="s">
-        <v>245</v>
-      </c>
-      <c r="G121" t="s">
-        <v>252</v>
+        <v>235</v>
+      </c>
+      <c r="G121" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="H121">
         <v>0</v>
@@ -4832,25 +4856,19 @@
     </row>
     <row r="122" spans="1:10" ht="15.75">
       <c r="A122" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B122" t="s">
         <v>11</v>
       </c>
       <c r="C122" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="D122" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="E122" t="s">
-        <v>254</v>
-      </c>
-      <c r="F122" t="s">
-        <v>245</v>
-      </c>
-      <c r="G122" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
       <c r="H122">
         <v>0</v>
@@ -4859,30 +4877,30 @@
         <v>15</v>
       </c>
       <c r="J122" t="s">
-        <v>96</v>
+        <v>65</v>
       </c>
     </row>
     <row r="123" spans="1:10" ht="15.75">
       <c r="A123" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B123" t="s">
         <v>11</v>
       </c>
       <c r="C123" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="D123" t="s">
+        <v>241</v>
+      </c>
+      <c r="E123" t="s">
+        <v>242</v>
+      </c>
+      <c r="F123" t="s">
         <v>243</v>
       </c>
-      <c r="E123" t="s">
-        <v>257</v>
-      </c>
-      <c r="F123" t="s">
-        <v>245</v>
-      </c>
       <c r="G123" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="H123">
         <v>0</v>
@@ -4891,30 +4909,30 @@
         <v>15</v>
       </c>
       <c r="J123" t="s">
-        <v>96</v>
+        <v>65</v>
       </c>
     </row>
     <row r="124" spans="1:10" ht="15.75">
       <c r="A124" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B124" t="s">
         <v>11</v>
       </c>
       <c r="C124" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="D124" t="s">
-        <v>260</v>
-      </c>
-      <c r="E124" s="1" t="s">
-        <v>261</v>
+        <v>246</v>
+      </c>
+      <c r="E124" t="s">
+        <v>247</v>
       </c>
       <c r="F124" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="G124" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="H124">
         <v>0</v>
@@ -4923,30 +4941,30 @@
         <v>15</v>
       </c>
       <c r="J124" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
     </row>
     <row r="125" spans="1:10" ht="15.75">
       <c r="A125" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B125" t="s">
         <v>11</v>
       </c>
       <c r="C125" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="D125" t="s">
-        <v>265</v>
+        <v>246</v>
       </c>
       <c r="E125" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="F125" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="G125" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="H125">
         <v>0</v>
@@ -4955,30 +4973,30 @@
         <v>15</v>
       </c>
       <c r="J125" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="126" spans="1:10" ht="15.75">
       <c r="A126" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B126" t="s">
         <v>11</v>
       </c>
       <c r="C126" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
       <c r="D126" t="s">
-        <v>265</v>
+        <v>246</v>
       </c>
       <c r="E126" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="F126" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="G126" t="s">
-        <v>271</v>
+        <v>255</v>
       </c>
       <c r="H126">
         <v>0</v>
@@ -4987,30 +5005,30 @@
         <v>15</v>
       </c>
       <c r="J126" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="127" spans="1:10" ht="15.75">
       <c r="A127" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B127" t="s">
         <v>11</v>
       </c>
       <c r="C127" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
       <c r="D127" t="s">
-        <v>265</v>
+        <v>246</v>
       </c>
       <c r="E127" t="s">
-        <v>273</v>
+        <v>257</v>
       </c>
       <c r="F127" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="G127" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="H127">
         <v>0</v>
@@ -5019,30 +5037,30 @@
         <v>15</v>
       </c>
       <c r="J127" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="128" spans="1:10" ht="15.75">
       <c r="A128" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B128" t="s">
         <v>11</v>
       </c>
       <c r="C128" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="D128" t="s">
-        <v>265</v>
+        <v>246</v>
       </c>
       <c r="E128" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
       <c r="F128" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="G128" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
       <c r="H128">
         <v>0</v>
@@ -5051,30 +5069,30 @@
         <v>15</v>
       </c>
       <c r="J128" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="129" spans="1:10" ht="15.75">
       <c r="A129" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B129" t="s">
         <v>11</v>
       </c>
       <c r="C129" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
       <c r="D129" t="s">
+        <v>263</v>
+      </c>
+      <c r="E129" t="s">
+        <v>264</v>
+      </c>
+      <c r="F129" t="s">
         <v>265</v>
       </c>
-      <c r="E129" t="s">
-        <v>279</v>
-      </c>
-      <c r="F129" t="s">
-        <v>267</v>
-      </c>
       <c r="G129" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="H129">
         <v>0</v>
@@ -5083,44 +5101,204 @@
         <v>15</v>
       </c>
       <c r="J129" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
     </row>
     <row r="130" spans="1:10" ht="15.75">
       <c r="A130" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B130" t="s">
         <v>11</v>
       </c>
       <c r="C130" t="s">
+        <v>267</v>
+      </c>
+      <c r="D130" t="s">
+        <v>268</v>
+      </c>
+      <c r="E130" t="s">
+        <v>269</v>
+      </c>
+      <c r="F130" t="s">
+        <v>270</v>
+      </c>
+      <c r="G130" t="s">
+        <v>271</v>
+      </c>
+      <c r="H130">
+        <v>0</v>
+      </c>
+      <c r="I130" t="s">
+        <v>15</v>
+      </c>
+      <c r="J130" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" ht="15.75">
+      <c r="A131" t="s">
+        <v>236</v>
+      </c>
+      <c r="B131" t="s">
+        <v>11</v>
+      </c>
+      <c r="C131" t="s">
+        <v>272</v>
+      </c>
+      <c r="D131" t="s">
+        <v>268</v>
+      </c>
+      <c r="E131" t="s">
+        <v>273</v>
+      </c>
+      <c r="F131" t="s">
+        <v>270</v>
+      </c>
+      <c r="G131" t="s">
+        <v>274</v>
+      </c>
+      <c r="H131">
+        <v>0</v>
+      </c>
+      <c r="I131" t="s">
+        <v>15</v>
+      </c>
+      <c r="J131" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" ht="15.75">
+      <c r="A132" t="s">
+        <v>236</v>
+      </c>
+      <c r="B132" t="s">
+        <v>11</v>
+      </c>
+      <c r="C132" t="s">
+        <v>275</v>
+      </c>
+      <c r="D132" t="s">
+        <v>268</v>
+      </c>
+      <c r="E132" t="s">
+        <v>276</v>
+      </c>
+      <c r="F132" t="s">
+        <v>270</v>
+      </c>
+      <c r="G132" t="s">
+        <v>277</v>
+      </c>
+      <c r="H132">
+        <v>0</v>
+      </c>
+      <c r="I132" t="s">
+        <v>15</v>
+      </c>
+      <c r="J132" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" ht="15.75">
+      <c r="A133" t="s">
+        <v>236</v>
+      </c>
+      <c r="B133" t="s">
+        <v>11</v>
+      </c>
+      <c r="C133" t="s">
+        <v>278</v>
+      </c>
+      <c r="D133" t="s">
+        <v>268</v>
+      </c>
+      <c r="E133" t="s">
+        <v>279</v>
+      </c>
+      <c r="F133" t="s">
+        <v>270</v>
+      </c>
+      <c r="G133" t="s">
+        <v>280</v>
+      </c>
+      <c r="H133">
+        <v>0</v>
+      </c>
+      <c r="I133" t="s">
+        <v>15</v>
+      </c>
+      <c r="J133" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" ht="15.75">
+      <c r="A134" t="s">
+        <v>236</v>
+      </c>
+      <c r="B134" t="s">
+        <v>11</v>
+      </c>
+      <c r="C134" t="s">
         <v>281</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D134" t="s">
+        <v>268</v>
+      </c>
+      <c r="E134" t="s">
         <v>282</v>
       </c>
-      <c r="E130" s="1" t="s">
+      <c r="F134" t="s">
+        <v>270</v>
+      </c>
+      <c r="G134" t="s">
         <v>283</v>
       </c>
-      <c r="F130" s="5" t="s">
+      <c r="H134">
+        <v>0</v>
+      </c>
+      <c r="I134" t="s">
+        <v>15</v>
+      </c>
+      <c r="J134" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" ht="15.75">
+      <c r="A135" t="s">
+        <v>236</v>
+      </c>
+      <c r="B135" t="s">
+        <v>11</v>
+      </c>
+      <c r="C135" t="s">
         <v>284</v>
       </c>
-      <c r="G130" t="s">
+      <c r="D135" t="s">
         <v>285</v>
       </c>
-      <c r="H130">
-        <v>0</v>
-      </c>
-      <c r="I130">
-        <v>8</v>
-      </c>
-      <c r="J130" t="s">
+      <c r="E135" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F135" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="G135" t="s">
+        <v>288</v>
+      </c>
+      <c r="H135">
+        <v>0</v>
+      </c>
+      <c r="I135" t="s">
+        <v>15</v>
+      </c>
+      <c r="J135" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K69" r:id="rId1" xr:uid="{709764D4-718C-4114-A0AC-ADB901EC24BF}"/>
+    <hyperlink ref="K72" r:id="rId1" xr:uid="{709764D4-718C-4114-A0AC-ADB901EC24BF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>